<commit_message>
Adicionando novo relatório e script
</commit_message>
<xml_diff>
--- a/dados/03_ferramentas_aws.xlsx
+++ b/dados/03_ferramentas_aws.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b755341190342fa/projetos/finops-automatic/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="11_E51D1B3A3542B0C86B301DCCA5C5AF74DE2DDE6B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4AC72F8-3410-4AEF-9258-AB80641FD3CB}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="11_E51D1B3A3542B0C86B301DCCA5C5AF74DE2DDE6B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37D68225-E0B2-4599-A0CF-F9856B3A4B91}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,21 +129,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <fill>
         <patternFill>
@@ -216,27 +202,6 @@
           <color indexed="64"/>
         </horizontal>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -436,7 +401,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -457,7 +422,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1234,9 +1198,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD9756EB-6BB2-40FD-8011-111D64BCE50D}" name="Tabela1" displayName="Tabela1" ref="A1:C6" totalsRowShown="0">
   <autoFilter ref="A1:C6" xr:uid="{DD9756EB-6BB2-40FD-8011-111D64BCE50D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4A50DF89-A5D7-49E8-851A-2BDF3A620AE6}" name="Ferramenta" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{6020B0AC-B960-4A59-BECA-7114B881DD31}" name="Status (Ativo/Inativo)" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B35C1D40-DA66-4254-8285-C32451F3D067}" name="Habilitado" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{4A50DF89-A5D7-49E8-851A-2BDF3A620AE6}" name="Ferramenta" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{6020B0AC-B960-4A59-BECA-7114B881DD31}" name="Status (Ativo/Inativo)" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B35C1D40-DA66-4254-8285-C32451F3D067}" name="Habilitado" dataDxfId="2">
       <calculatedColumnFormula>IF(B2="Ativo", 1, 0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1532,7 +1496,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1569,11 +1533,11 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1614,11 +1578,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Inativo"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Ativo"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
-      <formula>"Inativo"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>